<commit_message>
Added new documentation pages
</commit_message>
<xml_diff>
--- a/docs.xlsx
+++ b/docs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jegoussc/GitHub/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1046D9-0ACA-DD4D-83E8-B9BE1A6E68F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0903811F-991A-8549-B174-1701C465D420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{6A4DEADB-C4E1-8B4A-8160-CAD908C00F84}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>https://github.com/TeamMacLean/ENA_data_submission</t>
   </si>
@@ -62,6 +62,30 @@
   </si>
   <si>
     <t>https://github.com/TeamMacLean/ENA_data_upload</t>
+  </si>
+  <si>
+    <t>Introduction to the shell command line</t>
+  </si>
+  <si>
+    <t>For training TSL staff prior to HPC access</t>
+  </si>
+  <si>
+    <t>https://teammaclean.github.io/intro-shell-cmd-line/</t>
+  </si>
+  <si>
+    <t>https://teammaclean.github.io/tsl-shell-genomics/</t>
+  </si>
+  <si>
+    <t>Shell genomics</t>
+  </si>
+  <si>
+    <t>MSc course</t>
+  </si>
+  <si>
+    <t>https://teammaclean.github.io/tsl-wrangling-genomics/</t>
+  </si>
+  <si>
+    <t>Wrangling genomics</t>
   </si>
 </sst>
 </file>
@@ -413,13 +437,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB09864-110D-7C4F-BB2A-71AA26C113EE}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -452,6 +479,39 @@
       </c>
       <c r="C3" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>